<commit_message>
import data từ excel, viết API GET ALLCODE, fix lỗi 2 header UI
</commit_message>
<xml_diff>
--- a/Nodejs/design_db.xlsx
+++ b/Nodejs/design_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zCode\Web\BookingCare\Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D94EE0-36BB-402D-A735-7F2223AA97DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D305C130-9032-45FF-BC50-1CFA9460D4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14850" yWindow="465" windowWidth="13890" windowHeight="11385" xr2:uid="{5315B23F-9A75-4363-B747-EDE863C769D0}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{5315B23F-9A75-4363-B747-EDE863C769D0}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
   <si>
     <t>users</t>
   </si>
@@ -130,24 +130,12 @@
     <t>R3</t>
   </si>
   <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>DOCTOR</t>
-  </si>
-  <si>
-    <t>PATIENT</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
     <t>S1</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -157,15 +145,6 @@
     <t>S4</t>
   </si>
   <si>
-    <t>CONFIRMED</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>CANCEL</t>
-  </si>
-  <si>
     <t>TIME</t>
   </si>
   <si>
@@ -277,15 +256,6 @@
     <t>Bệnh nhân</t>
   </si>
   <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('ROLE','R1','ADMIN','Quản trị viên)</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('ROLE','R2','DOCTOR','Bác sĩ')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('ROLE','R3','PATIENT','Bệnh nhân')</t>
-  </si>
-  <si>
     <t>Lịch hẹn mới</t>
   </si>
   <si>
@@ -298,42 +268,6 @@
     <t>Đã hủy</t>
   </si>
   <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('STATUS','S1','NEW','Lịch hẹn mới')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('STATUS','S2','CONFIRMED','Đã xác nhận')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('STATUS','S3','DONE','Đã khám xong')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('STATUS','S4','CANCEL','Đã hủy')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T1','8:00 AM - 9:00 AM','8:00 - 9:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T2','9:00 AM - 10:00 AM','9:00 - 10:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T3','10:00 AM - 11:00 AM','10:00 - 11:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T4','11:00 AM - 00:00 PM','11:00 - 12:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T5','1:00 PM - 2:00 PM','13:00 - 14:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T6','2:00 PM - 3:00 PM','14:00 - 15:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T7','3:00 PM - 4:00 PM','15:00 - 16:00')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('TIME','T8','4:00 PM - 5:00 PM','16:00 - 17:00')</t>
-  </si>
-  <si>
     <t>POSITION</t>
   </si>
   <si>
@@ -379,19 +313,79 @@
     <t>Giáo sư</t>
   </si>
   <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('POSITION','P0','None','Bác sĩ')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('POSITION','P1','Master','Thạc sĩ')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('POSITION','P2','Doctor','Tiến sĩ')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('POSITION','P3','Associate Professor','Phó giáo sư')</t>
-  </si>
-  <si>
-    <t>INSERT INTO ALLCODE (type, key, value) values ('POSITION','P4','Professor','Giáo sư')</t>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>8:00 AM - 9:00 AM</t>
+  </si>
+  <si>
+    <t>9:00 AM - 10:00 AM</t>
+  </si>
+  <si>
+    <t>10:00 AM - 11:00 AM</t>
+  </si>
+  <si>
+    <t>11:00 AM - 00:00 PM</t>
+  </si>
+  <si>
+    <t>1:00 PM - 2:00 PM</t>
+  </si>
+  <si>
+    <t>2:00 PM - 3:00 PM</t>
+  </si>
+  <si>
+    <t>3:00 PM - 4:00 PM</t>
+  </si>
+  <si>
+    <t>4:00 PM - 5:00 PM</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>M, F, O</t>
   </si>
 </sst>
 </file>
@@ -447,10 +441,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,7 +765,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -837,7 +834,7 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -845,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -854,18 +851,18 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -880,13 +877,16 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -896,15 +896,15 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -921,13 +921,13 @@
         <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="K13" t="s">
         <v>4</v>
@@ -958,32 +958,32 @@
         <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -998,10 +998,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8230035-299C-47ED-A2F9-EA0CA60B5904}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,364 +1009,468 @@
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="84.7109375" customWidth="1"/>
+    <col min="5" max="5" width="131.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"');"</f>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R1','Admin','Quản trị viên');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E29" si="0">"INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"');"</f>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R2','Doctor','Bác sĩ');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R3','Patient','Bệnh nhân');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S1','New','Lịch hẹn mới');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S2','Confirmed','Đã xác nhận');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S3','Done','Đã khám xong');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S4','Cancel','Đã hủy');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T1','8:00 AM - 9:00 AM','8:00 - 9:00');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T2','9:00 AM - 10:00 AM','9:00 - 10:00');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T3','10:00 AM - 11:00 AM','10:00 - 11:00');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T4','11:00 AM - 00:00 PM','11:00 - 12:00');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T5','1:00 PM - 2:00 PM','13:00 - 14:00');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T6','2:00 PM - 3:00 PM','14:00 - 15:00');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T7','3:00 PM - 4:00 PM','15:00 - 16:00');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T8','4:00 PM - 5:00 PM','16:00 - 17:00');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P0','None','Bác sĩ');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P1','Master','Thạc sĩ');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P2','Doctor','Tiến sĩ');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P3','Associate Professor','Phó giáo sư');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C25" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D25" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P4','Professor','Giáo sư');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('GENDER','M','Male','Nam');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('GENDER','F','Female','Nữ');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('GENDER','O','Other','Khác');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tạo reducer, fire action, gọi API trong action, lưu data vào Redux
</commit_message>
<xml_diff>
--- a/Nodejs/design_db.xlsx
+++ b/Nodejs/design_db.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zCode\Web\BookingCare\Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D305C130-9032-45FF-BC50-1CFA9460D4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271EEC3D-A0EF-4F5F-AD2E-277C0ABB09A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{5315B23F-9A75-4363-B747-EDE863C769D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5315B23F-9A75-4363-B747-EDE863C769D0}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
     <sheet name="sample data" sheetId="2" r:id="rId2"/>
+    <sheet name="Redux" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="134">
   <si>
     <t>users</t>
   </si>
@@ -386,13 +387,87 @@
   </si>
   <si>
     <t>M, F, O</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Redux</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>&lt;= Components</t>
+  </si>
+  <si>
+    <t>Call Redux Events (actions)</t>
+  </si>
+  <si>
+    <t>Process data (eg: call API)</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>Reducers</t>
+  </si>
+  <si>
+    <t>Loops inside Actions (Switch case)</t>
+  </si>
+  <si>
+    <t>Saving data to State (Redux)</t>
+  </si>
+  <si>
+    <t>mapStateToProps</t>
+  </si>
+  <si>
+    <t>map data state Redux to Props (Component React)</t>
+  </si>
+  <si>
+    <t>(connect react-redux)</t>
+  </si>
+  <si>
+    <t>mapDispatchToProps</t>
+  </si>
+  <si>
+    <t>fire Redux actions with React's props</t>
+  </si>
+  <si>
+    <r>
+      <t>Saving data to Reducer (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dispatch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +481,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -441,13 +531,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,20 +855,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA722AB6-D3FC-4B01-9E14-8F81A226A6F1}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -820,7 +911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -837,7 +928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -854,7 +945,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>65</v>
       </c>
@@ -865,7 +956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -873,7 +964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -881,7 +972,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -889,12 +980,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
@@ -902,12 +993,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -933,7 +1024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -947,7 +1038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -961,7 +1052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>62</v>
       </c>
@@ -975,7 +1066,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>63</v>
       </c>
@@ -986,7 +1077,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>15</v>
       </c>
@@ -1004,15 +1095,15 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="131.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="131.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1029,7 +1120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1138,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R1','Admin','Quản trị viên');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1156,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R2','Doctor','Bác sĩ');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1083,13 +1174,13 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('ROLE','R3','Patient','Bệnh nhân');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1107,7 +1198,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S1','New','Lịch hẹn mới');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1216,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S2','Confirmed','Đã xác nhận');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1143,7 +1234,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S3','Done','Đã khám xong');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1161,13 +1252,13 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('STATUS','S4','Cancel','Đã hủy');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1276,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T1','8:00 AM - 9:00 AM','8:00 - 9:00');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1203,7 +1294,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T2','9:00 AM - 10:00 AM','9:00 - 10:00');</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1221,7 +1312,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T3','10:00 AM - 11:00 AM','10:00 - 11:00');</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1239,13 +1330,13 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T4','11:00 AM - 00:00 PM','11:00 - 12:00');</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1263,7 +1354,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T5','1:00 PM - 2:00 PM','13:00 - 14:00');</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1281,7 +1372,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T6','2:00 PM - 3:00 PM','14:00 - 15:00');</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1390,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T7','3:00 PM - 4:00 PM','15:00 - 16:00');</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1317,13 +1408,13 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('TIME','T8','4:00 PM - 5:00 PM','16:00 - 17:00');</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -1341,7 +1432,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P0','None','Bác sĩ');</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>77</v>
       </c>
@@ -1359,7 +1450,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P1','Master','Thạc sĩ');</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1468,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P2','Doctor','Tiến sĩ');</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>77</v>
       </c>
@@ -1395,7 +1486,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P3','Associate Professor','Phó giáo sư');</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1413,13 +1504,13 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('POSITION','P4','Professor','Giáo sư');</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>106</v>
       </c>
@@ -1437,7 +1528,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('GENDER','M','Male','Nam');</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>106</v>
       </c>
@@ -1455,7 +1546,7 @@
         <v>INSERT INTO ALLCODES (ALLCODES.type, ALLCODES.key, ALLCODES.valueEn, ALLCODES.valueVi) values ('GENDER','F','Female','Nữ');</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>106</v>
       </c>
@@ -1477,4 +1568,98 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EDD7AC-5E35-48A2-A796-6BB8A0A3B271}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" customWidth="1"/>
+    <col min="3" max="3" width="74" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>